<commit_message>
Unfinished- making array with all names in sheet
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -14,7 +14,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <si>
+    <t>mahi</t>
+  </si>
+  <si>
+    <t>dom</t>
+  </si>
+  <si>
+    <t>eric</t>
+  </si>
+  <si>
+    <t>john</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -265,7 +278,7 @@
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="topLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="14.43" defaultRowHeight="15"/>
@@ -275,6 +288,26 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2">
+      <c r="B2" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
adds new col for a new date
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,80 +1,97 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Form Responses 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <si>
-    <t>mahi</t>
-  </si>
-  <si>
-    <t>dom</t>
-  </si>
-  <si>
-    <t>eric</t>
-  </si>
-  <si>
-    <t>john</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
-  <numFmts count="8">
-    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
-    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);(&quot;$&quot;#,##0.00)"/>
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red](&quot;$&quot;#,##0.00)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* (#,##0);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* (#,##0);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* (#,##0.00);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* (#,##0.00);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt formatCode="m/d/yyyy h:mm:ss" numFmtId="164"/>
+    <numFmt formatCode="yyyy-mm-dd" numFmtId="165"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="4">
     <font>
       <name val="Arial"/>
       <color rgb="FF000000"/>
       <sz val="10"/>
     </font>
+    <font>
+      <name val="Arial"/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill patternType="solid"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left>
+        <color rgb="FF000000"/>
+      </left>
+      <right>
+        <color rgb="FF000000"/>
+      </right>
+      <top>
+        <color rgb="FF000000"/>
+      </top>
+      <bottom>
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal>
+        <color rgb="FF000000"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="10">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -272,43 +289,404 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" sqref="D11"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <selection activeCell="G5" pane="bottomLeft" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="14.43" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="2" min="1" width="21.57"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0">
-        <v>2</v>
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>First Name</t>
+        </is>
+      </c>
+      <c r="C1" s="9" t="n">
+        <v>43751</v>
       </c>
     </row>
     <row r="2">
-      <c r="B2" s="0" t="s">
-        <v>0</v>
+      <c r="A2" s="2" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B2" s="6" t="inlineStr">
+        <is>
+          <t>Eric Trostin</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="0" t="s">
-        <v>1</v>
+      <c r="A3" s="2" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B3" s="6" t="inlineStr">
+        <is>
+          <t>Nicholas Della Pesca</t>
+        </is>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="0" t="s">
-        <v>2</v>
+      <c r="A4" s="2" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>Justin Zhai</t>
+        </is>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="0" t="s">
-        <v>3</v>
+      <c r="A5" s="2" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B5" s="6" t="inlineStr">
+        <is>
+          <t>David Schmeltz</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B6" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lior Lichtenstein </t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B7" s="6" t="inlineStr">
+        <is>
+          <t>Taice Brenner</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B8" s="4" t="inlineStr">
+        <is>
+          <t>Ben Plaksienko</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B9" s="6" t="inlineStr">
+        <is>
+          <t>Andrew Keiser</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B10" s="6" t="inlineStr">
+        <is>
+          <t>John Madeja</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B11" s="6" t="inlineStr">
+        <is>
+          <t>Dominik Rozum</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B12" s="6" t="inlineStr">
+        <is>
+          <t>Nate Bresaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B13" s="6" t="inlineStr">
+        <is>
+          <t>Mark Shulkin</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B14" s="6" t="inlineStr">
+        <is>
+          <t>Michael Tomaszkowicz</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B15" s="6" t="inlineStr">
+        <is>
+          <t>Peter Redfern</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="5" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B16" s="6" t="inlineStr">
+        <is>
+          <t>Jaden Johnson</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="5" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B17" s="6" t="inlineStr">
+        <is>
+          <t>Mariyam Ahmed</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="5" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B18" s="6" t="inlineStr">
+        <is>
+          <t>Jacob Kramer</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="5" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B19" s="6" t="inlineStr">
+        <is>
+          <t>Steven Spivak</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="5" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B20" s="6" t="inlineStr">
+        <is>
+          <t>Alex Gorakine</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="5" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B21" s="6" t="inlineStr">
+        <is>
+          <t>Victor Jimenez</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="5" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B22" s="6" t="inlineStr">
+        <is>
+          <t>Jonathan Jorge</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="5" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B23" s="6" t="inlineStr">
+        <is>
+          <t>David Makarovsky</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="5" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B24" s="6" t="inlineStr">
+        <is>
+          <t>Kenneth Chiong</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="5" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B25" s="6" t="inlineStr">
+        <is>
+          <t>Brandon Kreitsch</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="5" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B26" s="6" t="inlineStr">
+        <is>
+          <t>Alina Smirnova</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="5" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B27" s="6" t="inlineStr">
+        <is>
+          <t>Brandon Yarvin</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="5" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B28" s="6" t="inlineStr">
+        <is>
+          <t>Michael Lisboa</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="5" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B29" s="6" t="inlineStr">
+        <is>
+          <t>Dariel Nunez</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="5" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B30" s="6" t="inlineStr">
+        <is>
+          <t>Antonio Faustina</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="5" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B31" s="6" t="inlineStr">
+        <is>
+          <t>Ethan Talanay</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="5" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B32" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Reisuke Ikeda </t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="5" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B33" s="6" t="inlineStr">
+        <is>
+          <t>Hargun Singh</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="5" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B34" s="6" t="inlineStr">
+        <is>
+          <t>Nafees Shaheed</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="5" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B35" s="6" t="inlineStr">
+        <is>
+          <t>Mahi Pasarkar</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="5" t="n">
+        <v>-7</v>
+      </c>
+      <c r="B36" s="6" t="inlineStr">
+        <is>
+          <t>Brandon Plaza</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0" header="0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup cellComments="atEnd" fitToHeight="0" orientation="landscape" pageOrder="overThenDown"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" pane="topLeft" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="14.43" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Got it to mark present!
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -298,10 +298,10 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
-      <selection activeCell="G5" pane="bottomLeft" sqref="G5"/>
+      <selection activeCell="C1" pane="bottomLeft" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="14.43" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="14.43" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="2" min="1" width="21.57"/>
   </cols>
@@ -312,23 +312,30 @@
           <t>First Name</t>
         </is>
       </c>
-      <c r="C1" s="9" t="n">
-        <v>43751</v>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>2019-10-13</t>
+        </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B2" s="6" t="inlineStr">
         <is>
           <t>Eric Trostin</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Present</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B3" s="6" t="inlineStr">
         <is>
@@ -338,7 +345,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B4" s="6" t="inlineStr">
         <is>
@@ -348,7 +355,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B5" s="6" t="inlineStr">
         <is>
@@ -358,7 +365,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B6" s="6" t="inlineStr">
         <is>
@@ -368,7 +375,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B7" s="6" t="inlineStr">
         <is>
@@ -378,7 +385,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B8" s="4" t="inlineStr">
         <is>
@@ -388,7 +395,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B9" s="6" t="inlineStr">
         <is>
@@ -398,7 +405,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B10" s="6" t="inlineStr">
         <is>
@@ -408,7 +415,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B11" s="6" t="inlineStr">
         <is>
@@ -418,7 +425,7 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B12" s="6" t="inlineStr">
         <is>
@@ -428,7 +435,7 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B13" s="6" t="inlineStr">
         <is>
@@ -438,7 +445,7 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B14" s="6" t="inlineStr">
         <is>
@@ -448,7 +455,7 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B15" s="6" t="inlineStr">
         <is>
@@ -458,7 +465,7 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B16" s="6" t="inlineStr">
         <is>
@@ -468,7 +475,7 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B17" s="6" t="inlineStr">
         <is>
@@ -478,7 +485,7 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B18" s="6" t="inlineStr">
         <is>
@@ -488,7 +495,7 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B19" s="6" t="inlineStr">
         <is>
@@ -498,7 +505,7 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B20" s="6" t="inlineStr">
         <is>
@@ -508,7 +515,7 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B21" s="6" t="inlineStr">
         <is>
@@ -518,7 +525,7 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B22" s="6" t="inlineStr">
         <is>
@@ -528,7 +535,7 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B23" s="6" t="inlineStr">
         <is>
@@ -538,7 +545,7 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B24" s="6" t="inlineStr">
         <is>
@@ -548,7 +555,7 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B25" s="6" t="inlineStr">
         <is>
@@ -558,7 +565,7 @@
     </row>
     <row r="26">
       <c r="A26" s="5" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B26" s="6" t="inlineStr">
         <is>
@@ -568,7 +575,7 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B27" s="6" t="inlineStr">
         <is>
@@ -578,7 +585,7 @@
     </row>
     <row r="28">
       <c r="A28" s="5" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B28" s="6" t="inlineStr">
         <is>
@@ -588,7 +595,7 @@
     </row>
     <row r="29">
       <c r="A29" s="5" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B29" s="6" t="inlineStr">
         <is>
@@ -598,7 +605,7 @@
     </row>
     <row r="30">
       <c r="A30" s="5" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B30" s="6" t="inlineStr">
         <is>
@@ -608,7 +615,7 @@
     </row>
     <row r="31">
       <c r="A31" s="5" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B31" s="6" t="inlineStr">
         <is>
@@ -618,7 +625,7 @@
     </row>
     <row r="32">
       <c r="A32" s="5" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B32" s="6" t="inlineStr">
         <is>
@@ -628,7 +635,7 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B33" s="6" t="inlineStr">
         <is>
@@ -638,7 +645,7 @@
     </row>
     <row r="34">
       <c r="A34" s="5" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B34" s="6" t="inlineStr">
         <is>
@@ -648,17 +655,22 @@
     </row>
     <row r="35">
       <c r="A35" s="5" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B35" s="6" t="inlineStr">
         <is>
           <t>Mahi Pasarkar</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Present</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="5" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="B36" s="6" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Made it faster, also added a message after signed in
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,121 +20,118 @@
     <t>First Name</t>
   </si>
   <si>
-    <t>2019-10-13</t>
+    <t>2019-10-15</t>
   </si>
   <si>
     <t>Eric Trostin</t>
   </si>
   <si>
+    <t>Nicholas Della Pesca</t>
+  </si>
+  <si>
+    <t>Justin Zhai</t>
+  </si>
+  <si>
+    <t>David Schmeltz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lior Lichtenstein </t>
+  </si>
+  <si>
+    <t>Taice Brenner</t>
+  </si>
+  <si>
+    <t>Ben Plaksienko</t>
+  </si>
+  <si>
+    <t>Andrew Keiser</t>
+  </si>
+  <si>
+    <t>John Madeja</t>
+  </si>
+  <si>
+    <t>Dominik Rozum</t>
+  </si>
+  <si>
+    <t>Nate Bresaz</t>
+  </si>
+  <si>
+    <t>Mark Shulkin</t>
+  </si>
+  <si>
+    <t>Michael Tomaszkowicz</t>
+  </si>
+  <si>
+    <t>Peter Redfern</t>
+  </si>
+  <si>
+    <t>Jaden Johnson</t>
+  </si>
+  <si>
+    <t>Mariyam Ahmed</t>
+  </si>
+  <si>
+    <t>Jacob Kramer</t>
+  </si>
+  <si>
+    <t>Steven Spivak</t>
+  </si>
+  <si>
+    <t>Alex Gorakine</t>
+  </si>
+  <si>
+    <t>Victor Jimenez</t>
+  </si>
+  <si>
+    <t>Jonathan Jorge</t>
+  </si>
+  <si>
+    <t>David Makarovsky</t>
+  </si>
+  <si>
+    <t>Kenneth Chiong</t>
+  </si>
+  <si>
+    <t>Brandon Kreitsch</t>
+  </si>
+  <si>
+    <t>Alina Smirnova</t>
+  </si>
+  <si>
+    <t>Brandon Yarvin</t>
+  </si>
+  <si>
+    <t>Michael Lisboa</t>
+  </si>
+  <si>
+    <t>Dariel Nunez</t>
+  </si>
+  <si>
+    <t>Antonio Faustina</t>
+  </si>
+  <si>
+    <t>Ethan Talanay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reisuke Ikeda </t>
+  </si>
+  <si>
+    <t>Hargun Singh</t>
+  </si>
+  <si>
+    <t>Nafees Shaheed</t>
+  </si>
+  <si>
+    <t>Mahi Pasarkar</t>
+  </si>
+  <si>
     <t>Present</t>
   </si>
   <si>
-    <t>Nicholas Della Pesca</t>
-  </si>
-  <si>
-    <t>Justin Zhai</t>
-  </si>
-  <si>
-    <t>David Schmeltz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lior Lichtenstein </t>
-  </si>
-  <si>
-    <t>Taice Brenner</t>
-  </si>
-  <si>
-    <t>Ben Plaksienko</t>
-  </si>
-  <si>
-    <t>Andrew Keiser</t>
-  </si>
-  <si>
-    <t>John Madeja</t>
-  </si>
-  <si>
-    <t>Dominik Rozum</t>
-  </si>
-  <si>
-    <t>Nate Bresaz</t>
-  </si>
-  <si>
-    <t>Mark Shulkin</t>
-  </si>
-  <si>
-    <t>Michael Tomaszkowicz</t>
-  </si>
-  <si>
-    <t>Peter Redfern</t>
-  </si>
-  <si>
-    <t>Jaden Johnson</t>
-  </si>
-  <si>
-    <t>Mariyam Ahmed</t>
-  </si>
-  <si>
-    <t>Jacob Kramer</t>
-  </si>
-  <si>
-    <t>Steven Spivak</t>
-  </si>
-  <si>
-    <t>Alex Gorakine</t>
-  </si>
-  <si>
-    <t>Victor Jimenez</t>
-  </si>
-  <si>
-    <t>Jonathan Jorge</t>
-  </si>
-  <si>
-    <t>David Makarovsky</t>
-  </si>
-  <si>
-    <t>Kenneth Chiong</t>
-  </si>
-  <si>
-    <t>Brandon Kreitsch</t>
-  </si>
-  <si>
-    <t>Alina Smirnova</t>
-  </si>
-  <si>
-    <t>Brandon Yarvin</t>
-  </si>
-  <si>
-    <t>Michael Lisboa</t>
-  </si>
-  <si>
-    <t>Dariel Nunez</t>
-  </si>
-  <si>
-    <t>Antonio Faustina</t>
-  </si>
-  <si>
-    <t>Ethan Talanay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reisuke Ikeda </t>
-  </si>
-  <si>
-    <t>Hargun Singh</t>
-  </si>
-  <si>
-    <t>Nafees Shaheed</t>
-  </si>
-  <si>
-    <t>Mahi Pasarkar</t>
-  </si>
-  <si>
-    <t>Present</t>
-  </si>
-  <si>
     <t>Brandon Plaza</t>
   </si>
   <si>
-    <t>John Doe</t>
+    <t>Joe Mama</t>
   </si>
   <si>
     <t>Present</t>
@@ -456,7 +453,7 @@
     </row>
     <row r="2">
       <c r="A2" s="10">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -464,274 +461,274 @@
     </row>
     <row r="3">
       <c r="A3" s="10">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="10">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="10">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="10">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="10">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="10">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="10">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="10">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="10">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="10">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="10">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="10">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="10">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="12">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="12">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="12">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="12">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="12">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="12">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="12">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="12">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="12">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="12">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="12">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="12">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="12">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="12">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="12">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="12">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="12">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="12">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="12">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="12">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="12">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>